<commit_message>
Add sequence diagram, wireframe V1
</commit_message>
<xml_diff>
--- a/hourly burndownwk16.xlsx
+++ b/hourly burndownwk16.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Li\Desktop\Ara\GD\BCCE301 Cooperative Education Project\Acdamic Folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Li\Desktop\Ara\GD\BCCE301DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042EF70F-7706-4ED8-BEE9-E134BDA1AB05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7229F452-8FAB-4CD4-98EE-2518F1AB22C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14243" yWindow="1590" windowWidth="21601" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -591,7 +591,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -752,71 +752,72 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="17" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="18" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="19" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1273,43 +1274,43 @@
                   <c:v>288</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>288</c:v>
+                  <c:v>274</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>288</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>288</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>288</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>288</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>288</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>288</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>288</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>288</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>288</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>288</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>288</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>288</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2076,43 +2077,43 @@
                   <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>144</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>144</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>144</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>144</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>144</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>144</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>144</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>144</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>144</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>144</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>144</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>144</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>144</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3891,13 +3892,13 @@
   <dimension ref="A1:I111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="23.1328125" customWidth="1"/>
-    <col min="2" max="2" width="24.3984375" customWidth="1"/>
+    <col min="1" max="1" width="23.06640625" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="24.59765625" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
@@ -3906,63 +3907,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="78"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="86"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1">
-      <c r="A2" s="79"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="81"/>
+      <c r="A2" s="87"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="89"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="23.25">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
+      <c r="B3" s="90"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="83"/>
-      <c r="B4" s="83"/>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
+      <c r="A4" s="90"/>
+      <c r="B4" s="90"/>
+      <c r="C4" s="90"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="90"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="13"/>
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82" t="s">
+      <c r="C5" s="83"/>
+      <c r="D5" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="82"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="14" t="s">
@@ -3982,268 +3983,268 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="96">
+      <c r="A7" s="81">
         <v>44067</v>
       </c>
-      <c r="B7" s="100">
+      <c r="B7" s="80">
         <v>0</v>
       </c>
-      <c r="C7" s="100">
+      <c r="C7" s="80">
         <v>0</v>
       </c>
-      <c r="D7" s="100">
+      <c r="D7" s="80">
         <v>288</v>
       </c>
-      <c r="E7" s="100">
+      <c r="E7" s="80">
         <f>D7</f>
         <v>288</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="96">
+      <c r="A8" s="76">
         <v>44074</v>
       </c>
-      <c r="B8" s="100">
+      <c r="B8" s="80">
         <v>24</v>
       </c>
-      <c r="C8" s="100">
-        <v>0</v>
-      </c>
-      <c r="D8" s="100">
+      <c r="C8" s="80">
+        <v>14</v>
+      </c>
+      <c r="D8" s="80">
         <f>D7-B8</f>
         <v>264</v>
       </c>
-      <c r="E8" s="100">
+      <c r="E8" s="80">
         <f>E7-C8</f>
-        <v>288</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="97">
+      <c r="A9" s="77">
         <v>44081</v>
       </c>
-      <c r="B9" s="100">
+      <c r="B9" s="80">
         <v>24</v>
       </c>
-      <c r="C9" s="100">
+      <c r="C9" s="80">
+        <v>24</v>
+      </c>
+      <c r="D9" s="80">
+        <f>D8-B9</f>
+        <v>240</v>
+      </c>
+      <c r="E9" s="80">
+        <f>(E8-C9)</f>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="77">
+        <v>44088</v>
+      </c>
+      <c r="B10" s="80">
+        <v>24</v>
+      </c>
+      <c r="C10" s="80">
+        <v>24</v>
+      </c>
+      <c r="D10" s="80">
+        <f>D9-B10</f>
+        <v>216</v>
+      </c>
+      <c r="E10" s="80">
+        <f t="shared" ref="E10:E20" si="0">E9-C10</f>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="77">
+        <v>44095</v>
+      </c>
+      <c r="B11" s="80">
+        <v>24</v>
+      </c>
+      <c r="C11" s="80">
         <v>0</v>
       </c>
-      <c r="D9" s="100">
-        <f t="shared" ref="D9:D12" si="0">D8-B9</f>
-        <v>240</v>
-      </c>
-      <c r="E9" s="100">
-        <f>(E8-C9)</f>
-        <v>288</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="97">
-        <v>44088</v>
-      </c>
-      <c r="B10" s="100">
+      <c r="D11" s="80">
+        <f>D10-B11</f>
+        <v>192</v>
+      </c>
+      <c r="E11" s="80">
+        <f t="shared" si="0"/>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="78">
+        <v>44102</v>
+      </c>
+      <c r="B12" s="80">
         <v>24</v>
       </c>
-      <c r="C10" s="100">
+      <c r="C12" s="80">
         <v>0</v>
       </c>
-      <c r="D10" s="100">
+      <c r="D12" s="80">
+        <f>D11-B12</f>
+        <v>168</v>
+      </c>
+      <c r="E12" s="80">
         <f t="shared" si="0"/>
-        <v>216</v>
-      </c>
-      <c r="E10" s="100">
-        <f t="shared" ref="E10:E20" si="1">E9-C10</f>
-        <v>288</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="97">
-        <v>44095</v>
-      </c>
-      <c r="B11" s="100">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="78">
+        <v>44109</v>
+      </c>
+      <c r="B13" s="80">
         <v>24</v>
       </c>
-      <c r="C11" s="100">
+      <c r="C13" s="80">
         <v>0</v>
       </c>
-      <c r="D11" s="100">
-        <f t="shared" si="0"/>
-        <v>192</v>
-      </c>
-      <c r="E11" s="100">
-        <f t="shared" si="1"/>
-        <v>288</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="98">
-        <v>44102</v>
-      </c>
-      <c r="B12" s="100">
-        <v>24</v>
-      </c>
-      <c r="C12" s="100">
-        <v>0</v>
-      </c>
-      <c r="D12" s="100">
-        <f t="shared" si="0"/>
-        <v>168</v>
-      </c>
-      <c r="E12" s="100">
-        <f t="shared" si="1"/>
-        <v>288</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="98">
-        <v>44109</v>
-      </c>
-      <c r="B13" s="100">
-        <v>24</v>
-      </c>
-      <c r="C13" s="100">
-        <v>0</v>
-      </c>
-      <c r="D13" s="100">
+      <c r="D13" s="80">
         <f>D12-B13</f>
         <v>144</v>
       </c>
-      <c r="E13" s="100">
+      <c r="E13" s="80">
         <f>E12-C13</f>
-        <v>288</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="98">
+      <c r="A14" s="78">
         <v>44116</v>
       </c>
-      <c r="B14" s="100">
+      <c r="B14" s="80">
         <v>24</v>
       </c>
-      <c r="C14" s="100">
+      <c r="C14" s="80">
         <v>0</v>
       </c>
-      <c r="D14" s="100">
-        <f t="shared" ref="D14:D20" si="2">D13-B14</f>
+      <c r="D14" s="80">
+        <f t="shared" ref="D14:D20" si="1">D13-B14</f>
         <v>120</v>
       </c>
-      <c r="E14" s="100">
+      <c r="E14" s="80">
+        <f t="shared" si="0"/>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="78">
+        <v>44123</v>
+      </c>
+      <c r="B15" s="80">
+        <v>24</v>
+      </c>
+      <c r="C15" s="80">
+        <v>0</v>
+      </c>
+      <c r="D15" s="80">
         <f t="shared" si="1"/>
-        <v>288</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="98">
-        <v>44123</v>
-      </c>
-      <c r="B15" s="100">
+        <v>96</v>
+      </c>
+      <c r="E15" s="80">
+        <f t="shared" si="0"/>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="78">
+        <v>44130</v>
+      </c>
+      <c r="B16" s="80">
         <v>24</v>
       </c>
-      <c r="C15" s="100">
+      <c r="C16" s="80">
         <v>0</v>
       </c>
-      <c r="D15" s="100">
-        <f t="shared" si="2"/>
-        <v>96</v>
-      </c>
-      <c r="E15" s="100">
+      <c r="D16" s="80">
         <f t="shared" si="1"/>
-        <v>288</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="98">
-        <v>44130</v>
-      </c>
-      <c r="B16" s="100">
+        <v>72</v>
+      </c>
+      <c r="E16" s="80">
+        <f t="shared" si="0"/>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="78">
+        <v>44137</v>
+      </c>
+      <c r="B17" s="80">
         <v>24</v>
       </c>
-      <c r="C16" s="100">
+      <c r="C17" s="80">
         <v>0</v>
       </c>
-      <c r="D16" s="100">
-        <f t="shared" si="2"/>
-        <v>72</v>
-      </c>
-      <c r="E16" s="100">
+      <c r="D17" s="80">
         <f t="shared" si="1"/>
-        <v>288</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="98">
-        <v>44137</v>
-      </c>
-      <c r="B17" s="100">
+        <v>48</v>
+      </c>
+      <c r="E17" s="80">
+        <f t="shared" si="0"/>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="79">
+        <v>44144</v>
+      </c>
+      <c r="B18" s="80">
         <v>24</v>
       </c>
-      <c r="C17" s="100">
+      <c r="C18" s="80">
         <v>0</v>
       </c>
-      <c r="D17" s="100">
-        <f t="shared" si="2"/>
-        <v>48</v>
-      </c>
-      <c r="E17" s="100">
+      <c r="D18" s="80">
         <f t="shared" si="1"/>
-        <v>288</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="99">
-        <v>44144</v>
-      </c>
-      <c r="B18" s="100">
         <v>24</v>
       </c>
-      <c r="C18" s="100">
+      <c r="E18" s="80">
+        <f t="shared" si="0"/>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="79">
+        <v>44151</v>
+      </c>
+      <c r="B19" s="80">
+        <v>24</v>
+      </c>
+      <c r="C19" s="80">
         <v>0</v>
       </c>
-      <c r="D18" s="100">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="E18" s="100">
+      <c r="D19" s="80">
         <f t="shared" si="1"/>
-        <v>288</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="99">
-        <v>44151</v>
-      </c>
-      <c r="B19" s="100">
-        <v>24</v>
-      </c>
-      <c r="C19" s="100">
         <v>0</v>
       </c>
-      <c r="D19" s="100">
-        <f t="shared" si="2"/>
+      <c r="E19" s="80">
+        <f t="shared" si="0"/>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="79">
+        <v>44158</v>
+      </c>
+      <c r="B20" s="80">
         <v>0</v>
       </c>
-      <c r="E19" s="100">
+      <c r="C20" s="80">
+        <v>0</v>
+      </c>
+      <c r="D20" s="80">
         <f t="shared" si="1"/>
-        <v>288</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="99">
-        <v>44158</v>
-      </c>
-      <c r="B20" s="100">
         <v>0</v>
       </c>
-      <c r="C20" s="100">
-        <v>0</v>
-      </c>
-      <c r="D20" s="100">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="100">
-        <f t="shared" si="1"/>
-        <v>288</v>
+      <c r="E20" s="80">
+        <f t="shared" si="0"/>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="12.75" customHeight="1">
@@ -4253,41 +4254,41 @@
       </c>
       <c r="C21" s="13">
         <f>SUM(C8:C20)</f>
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
     </row>
     <row r="23" spans="1:9" ht="23.25" customHeight="1">
-      <c r="A23" s="83" t="s">
+      <c r="A23" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="83"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="83"/>
-      <c r="E23" s="83"/>
+      <c r="B23" s="90"/>
+      <c r="C23" s="90"/>
+      <c r="D23" s="90"/>
+      <c r="E23" s="90"/>
     </row>
     <row r="24" spans="1:9" ht="23.25" customHeight="1">
-      <c r="A24" s="83"/>
-      <c r="B24" s="83"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="83"/>
-      <c r="E24" s="83"/>
+      <c r="A24" s="90"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="90"/>
+      <c r="D24" s="90"/>
+      <c r="E24" s="90"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="13"/>
-      <c r="B25" s="82" t="s">
+      <c r="B25" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="82"/>
-      <c r="D25" s="82" t="s">
+      <c r="C25" s="83"/>
+      <c r="D25" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="82"/>
-      <c r="F25" s="84"/>
-      <c r="G25" s="84"/>
-      <c r="H25" s="84"/>
-      <c r="I25" s="84"/>
+      <c r="E25" s="83"/>
+      <c r="F25" s="82"/>
+      <c r="G25" s="82"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="82"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="4" t="s">
@@ -4307,7 +4308,7 @@
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="96">
+      <c r="A27" s="76">
         <v>44067</v>
       </c>
       <c r="B27" s="11" t="s">
@@ -4324,14 +4325,14 @@
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="96">
+      <c r="A28" s="76">
         <v>44074</v>
       </c>
       <c r="B28" s="11">
         <v>11</v>
       </c>
       <c r="C28" s="7">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D28" s="11">
         <f>D27-B28</f>
@@ -4339,49 +4340,49 @@
       </c>
       <c r="E28" s="8">
         <f>E27-C28</f>
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="97">
+      <c r="A29" s="77">
         <v>44081</v>
       </c>
       <c r="B29" s="11">
         <v>11</v>
       </c>
       <c r="C29" s="7">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D29" s="11">
-        <f t="shared" ref="D29:D32" si="3">D28-B29</f>
+        <f>D28-B29</f>
         <v>122</v>
       </c>
       <c r="E29" s="8">
-        <f t="shared" ref="E29:E34" si="4">E28-C29</f>
-        <v>144</v>
+        <f t="shared" ref="E29:E34" si="2">E28-C29</f>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="97">
+      <c r="A30" s="77">
         <v>44088</v>
       </c>
       <c r="B30" s="11">
         <v>11</v>
       </c>
       <c r="C30" s="7">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D30" s="11">
-        <f t="shared" si="3"/>
+        <f>D29-B30</f>
         <v>111</v>
       </c>
       <c r="E30" s="8">
-        <f t="shared" si="4"/>
-        <v>144</v>
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="97">
+      <c r="A31" s="77">
         <v>44095</v>
       </c>
       <c r="B31" s="11">
@@ -4391,16 +4392,16 @@
         <v>0</v>
       </c>
       <c r="D31" s="11">
-        <f t="shared" si="3"/>
+        <f>D30-B31</f>
         <v>100</v>
       </c>
       <c r="E31" s="8">
-        <f t="shared" si="4"/>
-        <v>144</v>
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="98">
+      <c r="A32" s="78">
         <v>44102</v>
       </c>
       <c r="B32" s="11">
@@ -4410,16 +4411,16 @@
         <v>0</v>
       </c>
       <c r="D32" s="11">
-        <f t="shared" si="3"/>
+        <f>D31-B32</f>
         <v>88</v>
       </c>
       <c r="E32" s="8">
-        <f t="shared" si="4"/>
-        <v>144</v>
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="98">
+      <c r="A33" s="78">
         <v>44109</v>
       </c>
       <c r="B33" s="11">
@@ -4433,12 +4434,12 @@
         <v>77</v>
       </c>
       <c r="E33" s="8">
-        <f t="shared" si="4"/>
-        <v>144</v>
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="98">
+      <c r="A34" s="78">
         <v>44116</v>
       </c>
       <c r="B34" s="11">
@@ -4448,16 +4449,16 @@
         <v>0</v>
       </c>
       <c r="D34" s="11">
-        <f t="shared" ref="D34:D40" si="5">D33-B34</f>
+        <f t="shared" ref="D34:D40" si="3">D33-B34</f>
         <v>66</v>
       </c>
       <c r="E34" s="8">
-        <f t="shared" si="4"/>
-        <v>144</v>
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="98">
+      <c r="A35" s="78">
         <v>44123</v>
       </c>
       <c r="B35" s="11">
@@ -4467,16 +4468,16 @@
         <v>0</v>
       </c>
       <c r="D35" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="E35" s="8">
-        <f t="shared" ref="E35:E40" si="6">E34-C35</f>
-        <v>144</v>
+        <f t="shared" ref="E35:E40" si="4">E34-C35</f>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="98">
+      <c r="A36" s="78">
         <v>44130</v>
       </c>
       <c r="B36" s="11">
@@ -4486,16 +4487,16 @@
         <v>0</v>
       </c>
       <c r="D36" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>44</v>
       </c>
       <c r="E36" s="8">
-        <f t="shared" si="6"/>
-        <v>144</v>
+        <f t="shared" si="4"/>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="98">
+      <c r="A37" s="78">
         <v>44137</v>
       </c>
       <c r="B37" s="11">
@@ -4505,16 +4506,16 @@
         <v>0</v>
       </c>
       <c r="D37" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="E37" s="8">
-        <f t="shared" si="6"/>
-        <v>144</v>
+        <f t="shared" si="4"/>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="99">
+      <c r="A38" s="79">
         <v>44144</v>
       </c>
       <c r="B38" s="11">
@@ -4524,16 +4525,16 @@
         <v>0</v>
       </c>
       <c r="D38" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="E38" s="8">
-        <f t="shared" si="6"/>
-        <v>144</v>
+        <f t="shared" si="4"/>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="99">
+      <c r="A39" s="79">
         <v>44151</v>
       </c>
       <c r="B39" s="11">
@@ -4543,16 +4544,16 @@
         <v>0</v>
       </c>
       <c r="D39" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="E39" s="8">
-        <f t="shared" si="6"/>
-        <v>144</v>
+        <f t="shared" si="4"/>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="99">
+      <c r="A40" s="79">
         <v>44158</v>
       </c>
       <c r="B40" s="11">
@@ -4562,12 +4563,12 @@
         <v>0</v>
       </c>
       <c r="D40" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E40" s="8">
-        <f t="shared" si="6"/>
-        <v>144</v>
+        <f t="shared" si="4"/>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -4577,7 +4578,7 @@
       </c>
       <c r="C41" s="13">
         <f>SUM(C28:C40)</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
@@ -4589,7 +4590,7 @@
       </c>
       <c r="C42" s="13">
         <f>SUM(C21 + C41)</f>
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="D42" s="13"/>
       <c r="E42" s="13"/>
@@ -4703,10 +4704,10 @@
       <c r="A79" s="1"/>
     </row>
     <row r="94" spans="5:9">
-      <c r="F94" s="84"/>
-      <c r="G94" s="84"/>
-      <c r="H94" s="84"/>
-      <c r="I94" s="84"/>
+      <c r="F94" s="82"/>
+      <c r="G94" s="82"/>
+      <c r="H94" s="82"/>
+      <c r="I94" s="82"/>
     </row>
     <row r="95" spans="5:9">
       <c r="E95" s="1"/>
@@ -4761,6 +4762,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="A23:E24"/>
+    <mergeCell ref="A3:E4"/>
     <mergeCell ref="F94:G94"/>
     <mergeCell ref="H94:I94"/>
     <mergeCell ref="F25:G25"/>
@@ -4769,11 +4775,6 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A23:E24"/>
-    <mergeCell ref="A3:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="125" orientation="portrait" r:id="rId1"/>
@@ -4795,23 +4796,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="22.9" thickBot="1">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="94"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="100"/>
       <c r="K1" s="16"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="95"/>
-      <c r="B2" s="95"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
       <c r="C2" s="17" t="s">
         <v>16</v>
       </c>
@@ -4841,7 +4842,7 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="91" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="20">
@@ -4860,7 +4861,7 @@
       <c r="K3" s="73"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="87"/>
+      <c r="A4" s="93"/>
       <c r="B4" s="20">
         <v>27</v>
       </c>
@@ -4879,7 +4880,7 @@
       <c r="K4" s="73"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="85" t="s">
+      <c r="A5" s="91" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="20">
@@ -4898,7 +4899,7 @@
       <c r="K5" s="73"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="86"/>
+      <c r="A6" s="92"/>
       <c r="B6" s="20">
         <v>10</v>
       </c>
@@ -4915,7 +4916,7 @@
       <c r="K6" s="73"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="86"/>
+      <c r="A7" s="92"/>
       <c r="B7" s="20">
         <v>17</v>
       </c>
@@ -4934,7 +4935,7 @@
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="86"/>
+      <c r="A8" s="92"/>
       <c r="B8" s="20">
         <v>24</v>
       </c>
@@ -4953,7 +4954,7 @@
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="87"/>
+      <c r="A9" s="93"/>
       <c r="B9" s="20">
         <v>31</v>
       </c>
@@ -4972,7 +4973,7 @@
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="85" t="s">
+      <c r="A10" s="91" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="20">
@@ -4993,7 +4994,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="23.25">
-      <c r="A11" s="86"/>
+      <c r="A11" s="92"/>
       <c r="B11" s="20">
         <v>14</v>
       </c>
@@ -5014,7 +5015,7 @@
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="86"/>
+      <c r="A12" s="92"/>
       <c r="B12" s="20">
         <v>21</v>
       </c>
@@ -5033,7 +5034,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="34.9">
-      <c r="A13" s="87"/>
+      <c r="A13" s="93"/>
       <c r="B13" s="20">
         <v>28</v>
       </c>
@@ -5054,7 +5055,7 @@
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="85" t="s">
+      <c r="A14" s="91" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="20">
@@ -5075,7 +5076,7 @@
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="86"/>
+      <c r="A15" s="92"/>
       <c r="B15" s="20">
         <v>12</v>
       </c>
@@ -5094,7 +5095,7 @@
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="86"/>
+      <c r="A16" s="92"/>
       <c r="B16" s="20">
         <v>19</v>
       </c>
@@ -5113,7 +5114,7 @@
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="87"/>
+      <c r="A17" s="93"/>
       <c r="B17" s="47">
         <v>26</v>
       </c>
@@ -5134,7 +5135,7 @@
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="85" t="s">
+      <c r="A18" s="91" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="47">
@@ -5155,7 +5156,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="23.25">
-      <c r="A19" s="86"/>
+      <c r="A19" s="92"/>
       <c r="B19" s="47">
         <v>9</v>
       </c>
@@ -5176,7 +5177,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="23.25">
-      <c r="A20" s="86"/>
+      <c r="A20" s="92"/>
       <c r="B20" s="47">
         <v>16</v>
       </c>
@@ -5197,7 +5198,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="23.25">
-      <c r="A21" s="86"/>
+      <c r="A21" s="92"/>
       <c r="B21" s="20">
         <v>23</v>
       </c>
@@ -5216,7 +5217,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="23.25">
-      <c r="A22" s="87"/>
+      <c r="A22" s="93"/>
       <c r="B22" s="20">
         <v>30</v>
       </c>
@@ -5237,7 +5238,7 @@
       </c>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="88" t="s">
+      <c r="A23" s="94" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="20">
@@ -5260,7 +5261,7 @@
       <c r="K23" s="73"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="89"/>
+      <c r="A24" s="95"/>
       <c r="B24" s="20">
         <v>14</v>
       </c>
@@ -5277,7 +5278,7 @@
       <c r="K24" s="73"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="90"/>
+      <c r="A25" s="96"/>
       <c r="B25" s="20">
         <v>21</v>
       </c>

</xml_diff>